<commit_message>
creation of initial dvt/bring-up documents in anticipation of board arrival
</commit_message>
<xml_diff>
--- a/doc/design/pinouts.xlsx
+++ b/doc/design/pinouts.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10440" windowHeight="2511"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10440" windowHeight="2511" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pic32mx_pins" sheetId="2" r:id="rId1"/>
     <sheet name="pic32mx_funcs" sheetId="1" r:id="rId2"/>
+    <sheet name="connectors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="606">
   <si>
     <t>A1</t>
   </si>
@@ -1801,13 +1802,55 @@
   </si>
   <si>
     <t>P3_3V</t>
+  </si>
+  <si>
+    <t>Clicker 2 Endpoint</t>
+  </si>
+  <si>
+    <t>Clicker 2 to PICkit3 Adapter</t>
+  </si>
+  <si>
+    <t>PICkit3 Endpoint</t>
+  </si>
+  <si>
+    <t>2-PGC</t>
+  </si>
+  <si>
+    <t>4-MCLR</t>
+  </si>
+  <si>
+    <t>1-MCLR</t>
+  </si>
+  <si>
+    <t>5-VSS</t>
+  </si>
+  <si>
+    <t>1-VDD</t>
+  </si>
+  <si>
+    <t>2-VDD</t>
+  </si>
+  <si>
+    <t>3-VSS</t>
+  </si>
+  <si>
+    <t>4-PGD</t>
+  </si>
+  <si>
+    <t>5-PGC</t>
+  </si>
+  <si>
+    <t>3-PGD</t>
+  </si>
+  <si>
+    <t>6-PGM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1819,6 +1862,62 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1850,7 +1949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1865,6 +1964,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2311,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T101"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2323,10 +2438,9 @@
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="7" width="6.84375" customWidth="1"/>
     <col min="8" max="9" width="15.61328125" customWidth="1"/>
-    <col min="18" max="19" width="14.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="29.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="29.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>471</v>
       </c>
@@ -2369,14 +2483,8 @@
       <c r="O1" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>12</v>
       </c>
@@ -2421,14 +2529,8 @@
         <f>COUNTIF(Table3[[Usage (Clicker 2)]:[Usage (Clicker 2)]],"=*"&amp;O$1&amp;"*")</f>
         <v>13</v>
       </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>11</v>
       </c>
@@ -2469,17 +2571,8 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>590</v>
-      </c>
-      <c r="S3" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2520,17 +2613,8 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="Q4" s="1">
-        <v>2</v>
-      </c>
-      <c r="R4" t="s">
-        <v>579</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>19</v>
       </c>
@@ -2568,17 +2652,8 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="Q5" s="1">
-        <v>3</v>
-      </c>
-      <c r="R5" t="s">
-        <v>581</v>
-      </c>
-      <c r="S5" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>82</v>
       </c>
@@ -2616,17 +2691,8 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="Q6" s="1">
-        <v>4</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>580</v>
-      </c>
-      <c r="S6" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>78</v>
       </c>
@@ -2665,17 +2731,8 @@
         <f>SUM(O2:O6)</f>
         <v>16</v>
       </c>
-      <c r="Q7" s="1">
-        <v>5</v>
-      </c>
-      <c r="R7" t="s">
-        <v>586</v>
-      </c>
-      <c r="S7" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>80</v>
       </c>
@@ -2695,17 +2752,8 @@
       <c r="J8" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Q8" s="1">
-        <v>6</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="S8" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>79</v>
       </c>
@@ -2725,17 +2773,8 @@
       <c r="J9" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Q9" s="1">
-        <v>7</v>
-      </c>
-      <c r="R9" t="s">
-        <v>584</v>
-      </c>
-      <c r="S9" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>72</v>
       </c>
@@ -2758,17 +2797,8 @@
       <c r="J10" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Q10" s="1">
-        <v>8</v>
-      </c>
-      <c r="R10" t="s">
-        <v>583</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>33</v>
       </c>
@@ -2788,17 +2818,8 @@
       <c r="J11" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Q11" s="1">
-        <v>9</v>
-      </c>
-      <c r="R11" t="s">
-        <v>582</v>
-      </c>
-      <c r="S11" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>32</v>
       </c>
@@ -2818,17 +2839,8 @@
       <c r="J12" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Q12" s="1">
-        <v>10</v>
-      </c>
-      <c r="R12" t="s">
-        <v>483</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>44</v>
       </c>
@@ -2849,7 +2861,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>43</v>
       </c>
@@ -2870,7 +2882,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>42</v>
       </c>
@@ -2891,7 +2903,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>35</v>
       </c>
@@ -2912,7 +2924,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>34</v>
       </c>
@@ -2933,7 +2945,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>24</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>36</v>
       </c>
@@ -2980,9 +2992,8 @@
       <c r="J19" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="R19" s="9"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3012,7 +3023,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3030,9 +3041,8 @@
         <v>475</v>
       </c>
       <c r="J21" s="3"/>
-      <c r="R21" s="9"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>23</v>
       </c>
@@ -3051,7 +3061,7 @@
       </c>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>15</v>
       </c>
@@ -3079,7 +3089,7 @@
       </c>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>49</v>
       </c>
@@ -3101,7 +3111,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>50</v>
       </c>
@@ -3123,7 +3133,7 @@
       </c>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>58</v>
       </c>
@@ -3148,7 +3158,7 @@
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>59</v>
       </c>
@@ -3173,7 +3183,7 @@
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>66</v>
       </c>
@@ -3192,7 +3202,7 @@
       </c>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>67</v>
       </c>
@@ -3211,7 +3221,7 @@
       </c>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>18</v>
       </c>
@@ -3233,7 +3243,7 @@
       </c>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>40</v>
       </c>
@@ -3252,7 +3262,7 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>69</v>
       </c>
@@ -14072,4 +14082,213 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.53515625" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="11" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>590</v>
+      </c>
+      <c r="C3" t="s">
+        <v>591</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>598</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>595</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>601</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>581</v>
+      </c>
+      <c r="C5" t="s">
+        <v>574</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="C6" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>586</v>
+      </c>
+      <c r="C7" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="C8" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>584</v>
+      </c>
+      <c r="C9" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>583</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>582</v>
+      </c>
+      <c r="C11" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
very premliminary for half-duplex comm, data rec up on single ch
</commit_message>
<xml_diff>
--- a/doc/design/pinouts.xlsx
+++ b/doc/design/pinouts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\MS\doc\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\Thesis\doc\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14151,7 +14151,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>